<commit_message>
added DB3 and info_PLC
</commit_message>
<xml_diff>
--- a/DBs_PLC_300.xlsx
+++ b/DBs_PLC_300.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdenabeb\Google Drive\projects\demo_snap7_raspian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A385AF-3187-4BD1-9D8E-1A3FC81A364A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B34009-DC2E-4291-8AF5-CDEBE5064F67}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="1" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="3" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="DB2" sheetId="1" r:id="rId1"/>
     <sheet name="DB1" sheetId="2" r:id="rId2"/>
+    <sheet name="DB3" sheetId="3" r:id="rId3"/>
+    <sheet name="info_PLC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>DB_VAR</t>
   </si>
@@ -125,6 +127,114 @@
   </si>
   <si>
     <t>8.0</t>
+  </si>
+  <si>
+    <t>DB_DWORD</t>
+  </si>
+  <si>
+    <t>DWORD</t>
+  </si>
+  <si>
+    <t>DW#16#57</t>
+  </si>
+  <si>
+    <t>DB_Byte</t>
+  </si>
+  <si>
+    <t>B#16#39</t>
+  </si>
+  <si>
+    <t>DB_WORD</t>
+  </si>
+  <si>
+    <t>WORD</t>
+  </si>
+  <si>
+    <t>W#16#150</t>
+  </si>
+  <si>
+    <t>DB_DINT</t>
+  </si>
+  <si>
+    <t>DINT</t>
+  </si>
+  <si>
+    <t>L#300</t>
+  </si>
+  <si>
+    <t>DB_S5TIME</t>
+  </si>
+  <si>
+    <t>S5TIME</t>
+  </si>
+  <si>
+    <t>S5T#20MS</t>
+  </si>
+  <si>
+    <t>DB_TIME</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>T#14MS</t>
+  </si>
+  <si>
+    <t>DB_DATE</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>D#2018-5-30</t>
+  </si>
+  <si>
+    <t>DB_TOD</t>
+  </si>
+  <si>
+    <t>TIME_OF_DAY</t>
+  </si>
+  <si>
+    <t>TOD#12:30:15.000</t>
+  </si>
+  <si>
+    <t>DB_CHAR</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>'B'</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>26.0</t>
+  </si>
+  <si>
+    <t>IP_adress</t>
+  </si>
+  <si>
+    <t>10.32.0.95</t>
+  </si>
+  <si>
+    <t>rack</t>
+  </si>
+  <si>
+    <t>slot</t>
   </si>
 </sst>
 </file>
@@ -484,7 +594,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6587049-5806-44DB-AB47-46989DCA4B69}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,5 +854,239 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CC56E9-2CA5-43DE-8A0B-7B07F6D05F1C}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054A1064-456F-4C59-ACD3-1F866938F211}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added read and write for dword,byte,word,dint,time,date, time of dayand char
</commit_message>
<xml_diff>
--- a/DBs_PLC_300.xlsx
+++ b/DBs_PLC_300.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdenabeb\Google Drive\projects\demo_snap7_raspian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B34009-DC2E-4291-8AF5-CDEBE5064F67}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7606AEB-A5DE-427D-8F4A-CBF751DCEC42}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="3" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="8064" activeTab="2" xr2:uid="{F0EA8FC1-244E-4AA3-8AE3-B5F573F69DD9}"/>
   </bookViews>
   <sheets>
     <sheet name="DB2" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
   <si>
     <t>DB_VAR</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>slot</t>
+  </si>
+  <si>
+    <t>28.0</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,10 +863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CC56E9-2CA5-43DE-8A0B-7B07F6D05F1C}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,160 +892,171 @@
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1056,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054A1064-456F-4C59-ACD3-1F866938F211}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>